<commit_message>
solution blijkt niet goed meer te werken.
Ik heb alle sqlite dingen verwijderd en ben opnieuw begonnen. Solution was gebugged
</commit_message>
<xml_diff>
--- a/UrenRegistratie.xlsx
+++ b/UrenRegistratie.xlsx
@@ -687,7 +687,7 @@
   <dimension ref="A1:D175"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -723,7 +723,7 @@
       </c>
       <c r="D2" s="9">
         <f>SUM(C2:C172)</f>
-        <v>41.5</v>
+        <v>49.6</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -820,7 +820,7 @@
         <v>43357</v>
       </c>
       <c r="C12" s="5">
-        <v>0</v>
+        <v>8.1</v>
       </c>
       <c r="D12" s="8"/>
     </row>

</xml_diff>

<commit_message>
Logboek en urenregistratie bijgewerkt
</commit_message>
<xml_diff>
--- a/UrenRegistratie.xlsx
+++ b/UrenRegistratie.xlsx
@@ -687,7 +687,7 @@
   <dimension ref="A1:D175"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -723,7 +723,7 @@
       </c>
       <c r="D2" s="9">
         <f>SUM(C2:C172)</f>
-        <v>49.6</v>
+        <v>57.900000000000006</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -838,7 +838,7 @@
         <v>43360</v>
       </c>
       <c r="C14" s="5">
-        <v>0</v>
+        <v>8.3000000000000007</v>
       </c>
       <c r="D14" s="8"/>
     </row>

</xml_diff>

<commit_message>
uren registratie en logboek
bjhouden
</commit_message>
<xml_diff>
--- a/UrenRegistratie.xlsx
+++ b/UrenRegistratie.xlsx
@@ -687,7 +687,7 @@
   <dimension ref="A1:D175"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -723,7 +723,7 @@
       </c>
       <c r="D2" s="9">
         <f>SUM(C2:C172)</f>
-        <v>57.900000000000006</v>
+        <v>66.2</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -848,7 +848,7 @@
         <v>43361</v>
       </c>
       <c r="C15" s="5">
-        <v>0</v>
+        <v>8.3000000000000007</v>
       </c>
       <c r="D15" s="8"/>
     </row>

</xml_diff>